<commit_message>
Change label to Challenge
</commit_message>
<xml_diff>
--- a/biochar.xlsx
+++ b/biochar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokulgr/Library/CloudStorage/GoogleDrive-gokulr@alumni.princeton.edu/My Drive/Anjali_GR/Biochar/BEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715D18EB-C66A-9540-9329-F58F0D377C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E1FC04-B48E-9F49-A66E-B48917445CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{1518415A-8781-411C-82BA-68E1D4B75EB2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{1518415A-8781-411C-82BA-68E1D4B75EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,51 +50,6 @@
     <t>BEB 700</t>
   </si>
   <si>
-    <t>Transfer 0</t>
-  </si>
-  <si>
-    <t>Transfer 1</t>
-  </si>
-  <si>
-    <t>Transfer 2</t>
-  </si>
-  <si>
-    <t>Transfer 3</t>
-  </si>
-  <si>
-    <t>Transfer 4</t>
-  </si>
-  <si>
-    <t>Transfer 5</t>
-  </si>
-  <si>
-    <t>Transfer 6</t>
-  </si>
-  <si>
-    <t>Transfer 7</t>
-  </si>
-  <si>
-    <t>Transfer 8</t>
-  </si>
-  <si>
-    <t>Transfer 9</t>
-  </si>
-  <si>
-    <t>Transfer 10</t>
-  </si>
-  <si>
-    <t>Transfer 11</t>
-  </si>
-  <si>
-    <t>Transfer 12</t>
-  </si>
-  <si>
-    <t>Transfer 13</t>
-  </si>
-  <si>
-    <t>Transfer 14</t>
-  </si>
-  <si>
     <t>BEB 450_S</t>
   </si>
   <si>
@@ -102,6 +57,51 @@
   </si>
   <si>
     <t>BEB 700_S</t>
+  </si>
+  <si>
+    <t>Challenge 0</t>
+  </si>
+  <si>
+    <t>Challenge 1</t>
+  </si>
+  <si>
+    <t>Challenge 2</t>
+  </si>
+  <si>
+    <t>Challenge 3</t>
+  </si>
+  <si>
+    <t>Challenge 4</t>
+  </si>
+  <si>
+    <t>Challenge 5</t>
+  </si>
+  <si>
+    <t>Challenge 6</t>
+  </si>
+  <si>
+    <t>Challenge 7</t>
+  </si>
+  <si>
+    <t>Challenge 8</t>
+  </si>
+  <si>
+    <t>Challenge 9</t>
+  </si>
+  <si>
+    <t>Challenge 10</t>
+  </si>
+  <si>
+    <t>Challenge 11</t>
+  </si>
+  <si>
+    <t>Challenge 12</t>
+  </si>
+  <si>
+    <t>Challenge 13</t>
+  </si>
+  <si>
+    <t>Challenge 14</t>
   </si>
 </sst>
 </file>
@@ -527,18 +527,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>116.03733232856067</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>119.89955047475969</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>114.07139736307795</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>24.895473666202495</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>25.038103032059311</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4">
         <v>25.313583752989697</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>15.65</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>9.93</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>7.34</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
         <v>12.65</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>14.9</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
         <v>11.79</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
         <v>12.321338374622268</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4">
         <v>8.8563369304821826</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4">
         <v>11.602520841028062</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="17" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
         <v>12.46</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="18" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1">
         <v>9.5500000000000007</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
         <v>11.97</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="20" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>9.6199999999999992</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
         <v>13.58</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1">
         <v>10.53</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1">
         <v>8.0399999999999991</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1">
         <v>9.41</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1">
         <v>10.81</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="26" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B26" s="4">
         <v>48.661754855341599</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="27" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4">
         <v>33.148299581473538</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B28" s="4">
         <v>29.995540306845776</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B29" s="4">
         <v>34.194946664506105</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="30" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B30" s="4">
         <v>33.928578282214239</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B31" s="4">
         <v>29.465840818834153</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="32" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B32" s="1">
         <v>19.66</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1">
         <v>17.100000000000001</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
         <v>19.829999999999998</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B35" s="4">
         <v>45.436189588284371</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B36" s="4">
         <v>21.071244998277329</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="37" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B37" s="4">
         <v>33.511655235393491</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B38">
         <v>90.07</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B39">
         <v>61.3</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="40" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>88.81</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="41" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>13.23</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="42" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B42">
         <v>14.12</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="43" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>18.18</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="44" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>111.7</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="45" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B45">
         <v>163.27000000000001</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B46">
         <v>136.6</v>

</xml_diff>